<commit_message>
modifies daily uncorrected to have an adipose_clipped column to match with daily corrected
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_daily_uncorrected_passage.xlsx
+++ b/data-raw/metadata/yuba_daily_uncorrected_passage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7B1F1F-CEFE-1D47-A013-E9F1F3ED1161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4C08CE-D2A7-A843-8A48-74E3A486CB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18520" yWindow="-26800" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>biological_year</t>
   </si>
   <si>
-    <t>count_type</t>
-  </si>
-  <si>
     <t>vaki_operation</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Daily net upstream count of fish, uncorrected for periods of VAKI Riverwatcher non-operation.</t>
   </si>
   <si>
-    <t>Type of count. Levels = c("total fish", "adipose clipped fish"). "Total fish" includes adipose fin intact, adipose fin clipped, and adipose fin unidentified passing through the associated ladder; "adipose fin clipped fish" only includes fish with adipose fin clipped.</t>
-  </si>
-  <si>
     <t>Daily proportion of hours during which the VAKI Riverwatcher at the associated ladder was operational; values range from 0 (indicating 0 hours of operation) to 1 (indicating 24 hours of operation); inclusive.</t>
   </si>
   <si>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t>real</t>
+  </si>
+  <si>
+    <t>adipose_clipped</t>
+  </si>
+  <si>
+    <t>Whether or not the fish observed had a clipped adipose fin. Levels = c(TRUE, FALSE). If FALSE includes adipose fin intact and adipose fin unidentified; TRUE includes fish with adipose fin clipped.</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -259,7 +259,6 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -558,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>16</v>
@@ -602,7 +601,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>16</v>
@@ -618,13 +617,13 @@
       <c r="H3" s="14"/>
       <c r="I3" s="13"/>
       <c r="J3" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K3" s="13"/>
-      <c r="L3" s="21">
+      <c r="L3" s="14">
         <v>2004</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="14">
         <v>2022</v>
       </c>
       <c r="N3" s="1"/>
@@ -646,7 +645,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>27</v>
@@ -684,7 +683,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>14</v>
@@ -707,10 +706,10 @@
       <c r="I5" s="13"/>
       <c r="J5" s="14"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="21">
+      <c r="L5" s="14">
         <v>0</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="14">
         <v>539</v>
       </c>
       <c r="N5" s="1"/>
@@ -729,10 +728,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>27</v>
@@ -767,10 +766,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>14</v>
@@ -785,10 +784,10 @@
         <v>14</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="14"/>

</xml_diff>